<commit_message>
Added gmail url to config, added open/close gmail workflows
</commit_message>
<xml_diff>
--- a/Project2Final/Data/Config.xlsx
+++ b/Project2Final/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\JewlzAndTheBoyz-EmailCategorizationBot-P2\Project2Final\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\Project2Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4436683-6566-4C5C-84BC-C43D638A2C11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB43CD8C-6F55-4AED-9D22-8EB180378B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64410" yWindow="3300" windowWidth="17280" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="7050" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -125,12 +125,18 @@
   <si>
     <t>GsuiteBotCredentials</t>
   </si>
+  <si>
+    <t>GmailURL</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/?authuser=jewlzandtheboyz@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,6 +160,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,10 +184,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -185,8 +198,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,15 +517,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.578125" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -566,7 +581,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -577,7 +592,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1572,8 +1594,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{73A0C1D5-2347-4666-BDD6-360D4A87DFE8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1583,12 +1608,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1625,7 +1650,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2695,12 +2720,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.83984375" customWidth="1"/>
-    <col min="2" max="2" width="30.15625" customWidth="1"/>
-    <col min="3" max="3" width="60.26171875" customWidth="1"/>
-    <col min="4" max="26" width="65.41796875" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added additional queue add + Sentiment analysis
</commit_message>
<xml_diff>
--- a/Project2Final/Data/Config.xlsx
+++ b/Project2Final/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\Project2Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB43CD8C-6F55-4AED-9D22-8EB180378B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C8CAB2-C6BA-49D3-B07E-792FCFB25F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="7050" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>https://mail.google.com/mail/u/?authuser=jewlzandtheboyz@gmail.com</t>
+  </si>
+  <si>
+    <t>EmailInputQueueName</t>
+  </si>
+  <si>
+    <t>Sentiment Queue</t>
+  </si>
+  <si>
+    <t>Queue which the dispatcher puts email items into when sorting. sortEmail.xaml</t>
   </si>
 </sst>
 </file>
@@ -517,7 +526,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -600,7 +609,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>